<commit_message>
Modifico test de read_xlsx_table para evitar problemas con campos nulos
</commit_message>
<xml_diff>
--- a/tests/samples/read_table.xlsx
+++ b/tests/samples/read_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Plato</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">Aceitunas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gratis</t>
   </si>
 </sst>
 </file>
@@ -58,6 +61,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -142,15 +146,15 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.71428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -189,6 +193,9 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>7</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>8</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>15</v>

</xml_diff>

<commit_message>
COrrijo tests para lidiar mínimamente bien con archivos XLSX
</commit_message>
<xml_diff>
--- a/tests/samples/read_table.xlsx
+++ b/tests/samples/read_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Plato</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t xml:space="preserve">Aceitunas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gratis</t>
   </si>
 </sst>
 </file>
@@ -151,10 +148,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.0765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -193,9 +189,6 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>8</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>15</v>

</xml_diff>